<commit_message>
[update]: added excel functionality to main script
</commit_message>
<xml_diff>
--- a/websites.xlsx
+++ b/websites.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10" conformance="strict">
+<workbook xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2" conformance="strict">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10413"/>
   <workbookPr dateCompatibility="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/code/scraper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/daniel/code/Private-Equity-Python-Contact-Scraper-1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{747B0139-C76C-DA40-944D-6C53D21E8BAB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C1C06145-B379-B149-BF06-FBA60DB8E966}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="500" windowWidth="16340" windowHeight="10840"/>
+    <workbookView xWindow="16580" yWindow="14160" windowWidth="17020" windowHeight="6840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="3" uniqueCount="3">
+<sst xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" count="19" uniqueCount="13">
   <si>
     <t>https://www.newmountaincapital.com/</t>
   </si>
@@ -40,12 +40,42 @@
   </si>
   <si>
     <t>https://www.goldengatecap.com/</t>
+  </si>
+  <si>
+    <t>https://www.goldmansachs.com/</t>
+  </si>
+  <si>
+    <t>https://www.sfequitypartners.com/</t>
+  </si>
+  <si>
+    <t>https://www.skyknightcapital.com/team</t>
+  </si>
+  <si>
+    <t>https://www.serentcapital.com/team/</t>
+  </si>
+  <si>
+    <t>https://www.bannekerpartners.com/team</t>
+  </si>
+  <si>
+    <t>http://www.sandtoncapital.com/team</t>
+  </si>
+  <si>
+    <t>https://www.gipartners.com/team</t>
+  </si>
+  <si>
+    <t>https://www.marketsgroup.org/team</t>
+  </si>
+  <si>
+    <t>https://crimsoninvestment.com/our-team/</t>
+  </si>
+  <si>
+    <t>https://www.vistaequitypartners.com/about/team/</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
@@ -394,14 +424,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A13"/>
+  <dimension ref="A1:A19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -422,34 +452,84 @@
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A10" s="1"/>
+      <c r="A10" s="1" t="s">
+        <v>8</v>
+      </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A11" s="1"/>
+      <c r="A11" s="1" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A12" s="1"/>
+      <c r="A12" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.15">
-      <c r="A13" s="1"/>
+      <c r="A13" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <printOptions horizontalCentered="1"/>

</xml_diff>